<commit_message>
upd - organised folder + added new InSAR sites to excel data
</commit_message>
<xml_diff>
--- a/data/insar_points.xlsx
+++ b/data/insar_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PROJECTS\CURRENT\2021-004 SNC_Northern Road Link\InSAR\R_Analysis_MGW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5186B99-4F6D-48B4-B09F-3B1E78F5F7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1988E16-4F5F-4513-9958-3E908ED64FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="240" windowWidth="15660" windowHeight="11295" xr2:uid="{7E3CB24A-EC6F-429E-965D-FE4C47DB6002}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>26</t>
+  </si>
+  <si>
+    <t>tbd</t>
   </si>
 </sst>
 </file>
@@ -503,11 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665AD29B-C63E-4585-A566-57539D817CDE}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,87 +541,87 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>4997257</v>
+        <v>5004265</v>
       </c>
       <c r="B2" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C2" s="2">
-        <v>10</v>
+        <v>2017</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D2" s="2">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>4997257</v>
+        <v>5004265</v>
       </c>
       <c r="B3" s="2">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>4997257</v>
+        <v>5004265</v>
       </c>
       <c r="B4" s="2">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4997257</v>
+        <v>5004265</v>
       </c>
       <c r="B5" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>4997257</v>
+        <v>5004265</v>
       </c>
       <c r="B6" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,13 +629,13 @@
         <v>4997257</v>
       </c>
       <c r="B7" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -643,13 +646,13 @@
         <v>4997257</v>
       </c>
       <c r="B8" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
@@ -660,13 +663,13 @@
         <v>4997257</v>
       </c>
       <c r="B9" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -677,13 +680,13 @@
         <v>4997257</v>
       </c>
       <c r="B10" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
@@ -694,13 +697,13 @@
         <v>4997257</v>
       </c>
       <c r="B11" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
@@ -711,13 +714,13 @@
         <v>4997257</v>
       </c>
       <c r="B12" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>5</v>
@@ -728,13 +731,13 @@
         <v>4997257</v>
       </c>
       <c r="B13" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
@@ -745,12 +748,12 @@
         <v>4997257</v>
       </c>
       <c r="B14" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2">
         <v>20</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -759,16 +762,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>4997256</v>
+        <v>4997257</v>
       </c>
       <c r="B15" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C15" s="2">
-        <v>10</v>
+        <v>2020</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D15" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>5</v>
@@ -776,16 +779,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>4997256</v>
+        <v>4997257</v>
       </c>
       <c r="B16" s="2">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>5</v>
@@ -793,16 +796,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>4997256</v>
+        <v>4997257</v>
       </c>
       <c r="B17" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>5</v>
@@ -810,16 +813,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>4997256</v>
+        <v>4997257</v>
       </c>
       <c r="B18" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
@@ -827,16 +830,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>4997256</v>
+        <v>4997257</v>
       </c>
       <c r="B19" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2">
-        <v>18</v>
+      <c r="D19" s="3">
+        <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>5</v>
@@ -847,32 +850,32 @@
         <v>4997256</v>
       </c>
       <c r="B20" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C20" s="3" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C20" s="2">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>4997256</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>4997256</v>
-      </c>
-      <c r="B21" s="4">
-        <v>2019</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="4">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="2">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -881,13 +884,13 @@
         <v>4997256</v>
       </c>
       <c r="B22" s="2">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
@@ -898,13 +901,13 @@
         <v>4997256</v>
       </c>
       <c r="B23" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="2">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>5</v>
@@ -915,13 +918,13 @@
         <v>4997256</v>
       </c>
       <c r="B24" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>5</v>
@@ -932,32 +935,32 @@
         <v>4997256</v>
       </c>
       <c r="B25" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="2">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="4">
         <v>4997256</v>
       </c>
-      <c r="B26" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3">
-        <v>15</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="B26" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -966,13 +969,13 @@
         <v>4997256</v>
       </c>
       <c r="B27" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D27" s="2">
+        <v>20</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>5</v>
@@ -983,13 +986,13 @@
         <v>4997256</v>
       </c>
       <c r="B28" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="3">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D28" s="2">
+        <v>26</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>5</v>
@@ -997,203 +1000,203 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>5088845</v>
+        <v>4997256</v>
       </c>
       <c r="B29" s="2">
-        <v>2017</v>
-      </c>
-      <c r="C29" s="3">
-        <v>10</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>2020</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2">
+        <v>26</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>5088845</v>
+        <v>4997256</v>
       </c>
       <c r="B30" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D30" s="2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>5088845</v>
+        <v>4997256</v>
       </c>
       <c r="B31" s="2">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D31" s="3">
+        <v>15</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
+        <v>4997256</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>4997256</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>5088845</v>
       </c>
-      <c r="B32" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>5088845</v>
-      </c>
-      <c r="B33" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="5">
-        <v>18</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>5088845</v>
-      </c>
-      <c r="B34" s="4">
-        <v>2021</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="5">
-        <v>27</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="B34" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C34" s="3">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>5050228</v>
+        <v>5088845</v>
       </c>
       <c r="B35" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C35" s="2">
-        <v>11</v>
+        <v>2018</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D35" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>5050228</v>
+        <v>5088845</v>
       </c>
       <c r="B36" s="2">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="2">
-        <v>31</v>
+      <c r="D36" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>5050228</v>
+        <v>5088845</v>
       </c>
       <c r="B37" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="2">
+        <v>12</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>5088845</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="5">
         <v>18</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>5050228</v>
-      </c>
-      <c r="B38" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>14</v>
+      <c r="E38" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>5036155</v>
-      </c>
-      <c r="B39" s="2">
-        <v>2017</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="2">
-        <v>25</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>14</v>
+      <c r="A39" s="4">
+        <v>5088845</v>
+      </c>
+      <c r="B39" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="5">
+        <v>27</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>5036155</v>
+        <v>5050228</v>
       </c>
       <c r="B40" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>12</v>
+        <v>2016</v>
+      </c>
+      <c r="C40" s="2">
+        <v>11</v>
       </c>
       <c r="D40" s="2">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>14</v>
@@ -1201,16 +1204,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>5036155</v>
+        <v>5050228</v>
       </c>
       <c r="B41" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D41" s="2">
+        <v>31</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>14</v>
@@ -1218,7 +1221,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>5036155</v>
+        <v>5050228</v>
       </c>
       <c r="B42" s="2">
         <v>2019</v>
@@ -1227,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="D42" s="2">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>14</v>
@@ -1235,7 +1238,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>5036155</v>
+        <v>5050228</v>
       </c>
       <c r="B43" s="2">
         <v>2021</v>
@@ -1252,87 +1255,87 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>5247373</v>
+        <v>5036155</v>
       </c>
       <c r="B44" s="2">
         <v>2017</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="3">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="D44" s="2">
+        <v>25</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>5247373</v>
+        <v>5036155</v>
       </c>
       <c r="B45" s="2">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D45" s="2">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>5247373</v>
+        <v>5036155</v>
       </c>
       <c r="B46" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>5247373</v>
+        <v>5036155</v>
       </c>
       <c r="B47" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D47" s="2">
+        <v>25</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>5247373</v>
+        <v>5036155</v>
       </c>
       <c r="B48" s="2">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="2">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,13 +1343,13 @@
         <v>5247373</v>
       </c>
       <c r="B49" s="2">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>10</v>
+      <c r="D49" s="3">
+        <v>23</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>15</v>
@@ -1357,13 +1360,13 @@
         <v>5247373</v>
       </c>
       <c r="B50" s="2">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D50" s="2">
+        <v>21</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>15</v>
@@ -1374,13 +1377,13 @@
         <v>5247373</v>
       </c>
       <c r="B51" s="2">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>15</v>
@@ -1388,10 +1391,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>5050253</v>
+        <v>5247373</v>
       </c>
       <c r="B52" s="2">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>12</v>
@@ -1400,46 +1403,46 @@
         <v>8</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>5050253</v>
+        <v>5247373</v>
       </c>
       <c r="B53" s="2">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D53" s="2">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>5050253</v>
+        <v>5247373</v>
       </c>
       <c r="B54" s="2">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="3">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>5050253</v>
+        <v>5247373</v>
       </c>
       <c r="B55" s="2">
         <v>2021</v>
@@ -1448,49 +1451,49 @@
         <v>12</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>5050253</v>
+        <v>5247373</v>
       </c>
       <c r="B56" s="2">
         <v>2021</v>
       </c>
-      <c r="C56" s="2">
-        <v>10</v>
+      <c r="C56" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>4934110</v>
+        <v>5050253</v>
       </c>
       <c r="B57" s="2">
         <v>2017</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="3">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>4934110</v>
+        <v>5050253</v>
       </c>
       <c r="B58" s="2">
         <v>2017</v>
@@ -1498,62 +1501,62 @@
       <c r="C58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>10</v>
+      <c r="D58" s="2">
+        <v>11</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>4934110</v>
+        <v>5050253</v>
       </c>
       <c r="B59" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="2">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="D59" s="3">
+        <v>16</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>4934110</v>
+        <v>5050253</v>
       </c>
       <c r="B60" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="2">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>4934110</v>
+        <v>5050253</v>
       </c>
       <c r="B61" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="2">
-        <v>13</v>
+        <v>2021</v>
+      </c>
+      <c r="C61" s="2">
+        <v>10</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1561,13 +1564,13 @@
         <v>4934110</v>
       </c>
       <c r="B62" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="3">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>15</v>
@@ -1578,13 +1581,13 @@
         <v>4934110</v>
       </c>
       <c r="B63" s="2">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="2">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>15</v>
@@ -1595,13 +1598,13 @@
         <v>4934110</v>
       </c>
       <c r="B64" s="2">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="3">
-        <v>13</v>
+      <c r="D64" s="2">
+        <v>25</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>15</v>
@@ -1612,13 +1615,13 @@
         <v>4934110</v>
       </c>
       <c r="B65" s="2">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>10</v>
+      <c r="D65" s="2">
+        <v>25</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>15</v>
@@ -1629,13 +1632,13 @@
         <v>4934110</v>
       </c>
       <c r="B66" s="2">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>7</v>
+      <c r="D66" s="2">
+        <v>13</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>15</v>
@@ -1646,13 +1649,13 @@
         <v>4934110</v>
       </c>
       <c r="B67" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="D67" s="3">
+        <v>17</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>15</v>
@@ -1660,16 +1663,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>4927070</v>
+        <v>4934110</v>
       </c>
       <c r="B68" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C68" s="3">
-        <v>11</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>6</v>
+        <v>2020</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="2">
+        <v>28</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>15</v>
@@ -1677,70 +1680,70 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>4927070</v>
+        <v>4934110</v>
       </c>
       <c r="B69" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="3">
         <v>13</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>4927070</v>
+        <v>4934110</v>
       </c>
       <c r="B70" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="2">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>4927070</v>
+        <v>4934110</v>
       </c>
       <c r="B71" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="2">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>4927070</v>
+        <v>4934110</v>
       </c>
       <c r="B72" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" s="2">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,16 +1751,16 @@
         <v>4927070</v>
       </c>
       <c r="B73" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D73" s="2">
-        <v>18</v>
+        <v>2016</v>
+      </c>
+      <c r="C73" s="3">
+        <v>11</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,13 +1768,13 @@
         <v>4927070</v>
       </c>
       <c r="B74" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="2">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>11</v>
@@ -1782,13 +1785,13 @@
         <v>4927070</v>
       </c>
       <c r="B75" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D75" s="2">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>11</v>
@@ -1799,13 +1802,13 @@
         <v>4927070</v>
       </c>
       <c r="B76" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D76" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>11</v>
@@ -1816,13 +1819,13 @@
         <v>4927070</v>
       </c>
       <c r="B77" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D77" s="2">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>11</v>
@@ -1833,13 +1836,13 @@
         <v>4927070</v>
       </c>
       <c r="B78" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D78" s="2">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>11</v>
@@ -1850,13 +1853,13 @@
         <v>4927070</v>
       </c>
       <c r="B79" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D79" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>11</v>
@@ -1867,13 +1870,13 @@
         <v>4927070</v>
       </c>
       <c r="B80" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D80" s="2">
+        <v>13</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>11</v>
@@ -1884,13 +1887,13 @@
         <v>4927070</v>
       </c>
       <c r="B81" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D81" s="2">
+        <v>13</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>11</v>
@@ -1901,13 +1904,13 @@
         <v>4927070</v>
       </c>
       <c r="B82" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D82" s="2">
+        <v>15</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>11</v>
@@ -1918,13 +1921,13 @@
         <v>4927070</v>
       </c>
       <c r="B83" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D83" s="2">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>11</v>
@@ -1935,13 +1938,13 @@
         <v>4927070</v>
       </c>
       <c r="B84" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="2">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>11</v>
@@ -1949,87 +1952,87 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>4912985</v>
+        <v>4927070</v>
       </c>
       <c r="B85" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="2">
-        <v>15</v>
+      <c r="D85" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>4912985</v>
+        <v>4927070</v>
       </c>
       <c r="B86" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D86" s="2">
-        <v>13</v>
+      <c r="D86" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>4912985</v>
+        <v>4927070</v>
       </c>
       <c r="B87" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>4912985</v>
+        <v>4927070</v>
       </c>
       <c r="B88" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="3">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="D88" s="2">
+        <v>21</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>4912985</v>
+        <v>4927070</v>
       </c>
       <c r="B89" s="2">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D89" s="2">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2037,13 +2040,13 @@
         <v>4912985</v>
       </c>
       <c r="B90" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D90" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>18</v>
@@ -2054,13 +2057,13 @@
         <v>4912985</v>
       </c>
       <c r="B91" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C91" s="3">
-        <v>10</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>16</v>
+        <v>2017</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="2">
+        <v>13</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>18</v>
@@ -2071,13 +2074,13 @@
         <v>4912985</v>
       </c>
       <c r="B92" s="2">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>18</v>
@@ -2088,13 +2091,13 @@
         <v>4912985</v>
       </c>
       <c r="B93" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D93" s="3">
+        <v>24</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>18</v>
@@ -2105,13 +2108,13 @@
         <v>4912985</v>
       </c>
       <c r="B94" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" s="3">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="D94" s="2">
+        <v>26</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>18</v>
@@ -2122,13 +2125,13 @@
         <v>4912985</v>
       </c>
       <c r="B95" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D95" s="2">
+        <v>14</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>18</v>
@@ -2139,13 +2142,13 @@
         <v>4912985</v>
       </c>
       <c r="B96" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>12</v>
+        <v>2019</v>
+      </c>
+      <c r="C96" s="3">
+        <v>10</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>18</v>
@@ -2153,87 +2156,87 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>4818002</v>
+        <v>4912985</v>
       </c>
       <c r="B97" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C97" s="2">
-        <v>10</v>
-      </c>
-      <c r="D97" s="3">
-        <v>11</v>
+        <v>2020</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>4818002</v>
+        <v>4912985</v>
       </c>
       <c r="B98" s="2">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>4818002</v>
+        <v>4912985</v>
       </c>
       <c r="B99" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D99" s="2">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D99" s="3">
+        <v>14</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>4818002</v>
+        <v>4912985</v>
       </c>
       <c r="B100" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D100" s="2">
-        <v>21</v>
+      <c r="D100" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>4818002</v>
+        <v>4912985</v>
       </c>
       <c r="B101" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D101" s="2">
-        <v>25</v>
+      <c r="D101" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2241,13 +2244,13 @@
         <v>4818002</v>
       </c>
       <c r="B102" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" s="2">
-        <v>26</v>
+        <v>2016</v>
+      </c>
+      <c r="C102" s="2">
+        <v>10</v>
+      </c>
+      <c r="D102" s="3">
+        <v>11</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>11</v>
@@ -2258,13 +2261,13 @@
         <v>4818002</v>
       </c>
       <c r="B103" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="2">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>11</v>
@@ -2275,13 +2278,13 @@
         <v>4818002</v>
       </c>
       <c r="B104" s="2">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D104" s="2">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>11</v>
@@ -2292,13 +2295,13 @@
         <v>4818002</v>
       </c>
       <c r="B105" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D105" s="2">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>11</v>
@@ -2309,13 +2312,13 @@
         <v>4818002</v>
       </c>
       <c r="B106" s="2">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D106" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>11</v>
@@ -2326,13 +2329,13 @@
         <v>4818002</v>
       </c>
       <c r="B107" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D107" s="2">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>11</v>
@@ -2343,13 +2346,13 @@
         <v>4818002</v>
       </c>
       <c r="B108" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D108" s="2">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>11</v>
@@ -2360,15 +2363,100 @@
         <v>4818002</v>
       </c>
       <c r="B109" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" s="2">
+        <v>30</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>4818002</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="2">
+        <v>26</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>4818002</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="2">
+        <v>5</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>4818002</v>
+      </c>
+      <c r="B112" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" s="2">
         <v>16</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="E112" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>4818002</v>
+      </c>
+      <c r="B113" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113" s="2">
+        <v>26</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>4818002</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>